<commit_message>
Updated for end of semester
</commit_message>
<xml_diff>
--- a/Other Files/semester_reviews.xlsx
+++ b/Other Files/semester_reviews.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Miles/Documents/GitHub/miles-woollacott.github.io/Other Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D06AD1D-E607-A449-9432-0E9B2585F458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6CEE23-BD8E-6040-8D3F-881E7715EEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="1520" windowWidth="27240" windowHeight="16440" xr2:uid="{44B5C916-B487-F044-8F02-9782C62100F0}"/>
+    <workbookView xWindow="3000" yWindow="1520" windowWidth="27240" windowHeight="16440" xr2:uid="{44B5C916-B487-F044-8F02-9782C62100F0}"/>
   </bookViews>
   <sheets>
     <sheet name="semester_reviews" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Number</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Course</t>
+  </si>
+  <si>
+    <t>Spring 2025</t>
   </si>
 </sst>
 </file>
@@ -920,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF17B1FA-0F13-CA45-BAB6-5EF19AE71218}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1149,6 +1152,64 @@
       </c>
       <c r="I7">
         <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>